<commit_message>
added headshots and linkedin links, added graphs for economic tab on income, unemployment and retail sales. will see if i can add more tomorrow
</commit_message>
<xml_diff>
--- a/shinyApp/data/climate-floyd-county-usClimateData.xlsx
+++ b/shinyApp/data/climate-floyd-county-usClimateData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Floyd-County/DSPG_Floyd/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Floyd-County/DSPG_Floyd/shinyApp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40D79D6F-A906-1040-B584-2539508E16AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D6D850-4816-6640-9480-3A5736F68760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{8061D20D-E7C3-C24A-9175-C9976E60C2A4}"/>
+    <workbookView xWindow="2960" yWindow="500" windowWidth="10000" windowHeight="16940" xr2:uid="{8061D20D-E7C3-C24A-9175-C9976E60C2A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>